<commit_message>
Update distribution_report to use distribution_id instead of authorization_id
</commit_message>
<xml_diff>
--- a/app/config/tables/distribution_reports/forms/distribution_reports/distribution_reports.xlsx
+++ b/app/config/tables/distribution_reports/forms/distribution_reports/distribution_reports.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/tables/distribution_reports/forms/distribution_reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\Documents\oriredcross\app-designer\app\config\tables\distribution_reports\forms\distribution_reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="994" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16215" tabRatio="994" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -98,9 +98,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>authorization_id</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -126,12 +123,15 @@
   </si>
   <si>
     <t>date_created</t>
+  </si>
+  <si>
+    <t>distribution_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -416,6 +416,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -749,22 +752,22 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="33.125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="35.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="44.375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.375" style="5" customWidth="1"/>
     <col min="5" max="5" width="34.5" style="5" customWidth="1"/>
     <col min="6" max="6" width="34.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="1"/>
+    <col min="7" max="7" width="30.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -778,13 +781,13 @@
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="9"/>
@@ -792,7 +795,7 @@
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
       <c r="E3" s="9"/>
@@ -801,7 +804,7 @@
       <c r="H3" s="10"/>
       <c r="I3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C4" s="13"/>
       <c r="D4" s="14"/>
       <c r="F4"/>
@@ -809,7 +812,7 @@
       <c r="H4"/>
       <c r="I4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="15"/>
       <c r="C5" s="13"/>
       <c r="D5" s="14"/>
@@ -819,7 +822,7 @@
       <c r="H5"/>
       <c r="I5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="16"/>
       <c r="B6" s="17"/>
       <c r="C6" s="18"/>
@@ -830,7 +833,7 @@
       <c r="H6"/>
       <c r="I6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="16"/>
       <c r="B7" s="17"/>
       <c r="C7" s="18"/>
@@ -841,19 +844,19 @@
       <c r="H7"/>
       <c r="I7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C10" s="13"/>
       <c r="D10" s="14"/>
       <c r="F10"/>
@@ -861,7 +864,7 @@
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="13"/>
       <c r="D11" s="14"/>
       <c r="F11"/>
@@ -869,7 +872,7 @@
       <c r="H11"/>
       <c r="I11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" s="13"/>
       <c r="D12" s="14"/>
       <c r="F12"/>
@@ -877,7 +880,7 @@
       <c r="H12"/>
       <c r="I12"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" s="14"/>
       <c r="E13"/>
       <c r="F13"/>
@@ -885,28 +888,28 @@
       <c r="H13"/>
       <c r="I13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" s="14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" s="14"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" s="14"/>
       <c r="E16"/>
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D17" s="14"/>
       <c r="E17"/>
       <c r="F17"/>
@@ -914,14 +917,14 @@
       <c r="H17"/>
       <c r="I17"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="E18"/>
       <c r="F18"/>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="20"/>
       <c r="B19" s="21"/>
       <c r="C19" s="22"/>
@@ -929,7 +932,7 @@
       <c r="E19"/>
       <c r="I19"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -940,7 +943,7 @@
       <c r="H20"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="26"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -951,20 +954,20 @@
       <c r="H21"/>
       <c r="I21"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D24" s="14"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="24"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -975,7 +978,7 @@
       <c r="H25"/>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="20"/>
       <c r="B26"/>
       <c r="C26" s="25"/>
@@ -986,7 +989,7 @@
       <c r="H26"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="26"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -997,10 +1000,10 @@
       <c r="H27"/>
       <c r="I27"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D28" s="14"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C29" s="13"/>
       <c r="D29" s="14"/>
       <c r="F29"/>
@@ -1008,14 +1011,14 @@
       <c r="H29"/>
       <c r="I29"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D30" s="14"/>
       <c r="I30"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I31"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -1034,14 +1037,14 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.5" style="27" customWidth="1"/>
-    <col min="2" max="2" width="33.1640625" style="28" customWidth="1"/>
-    <col min="3" max="3" width="39.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="39.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>4</v>
       </c>
@@ -1052,16 +1055,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
         <v>8</v>
       </c>
@@ -1070,22 +1073,22 @@
       </c>
       <c r="C3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="27" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="27" t="s">
         <v>10</v>
       </c>
       <c r="B5"/>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1099,17 +1102,17 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
-    <col min="2" max="2" width="53.1640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="8.875" style="2"/>
+    <col min="2" max="2" width="53.125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1118,52 +1121,52 @@
       </c>
       <c r="C1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1180,9 +1183,9 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>11</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>

</xml_diff>